<commit_message>
Added FME workspace for CityGML and updated Excel
</commit_message>
<xml_diff>
--- a/QualityRules_CityGML.xlsx
+++ b/QualityRules_CityGML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATURUNEN\Work Folders\FME+DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFFDE6B-1F3A-451C-A402-6B2357230EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F11225-C68A-403C-B267-941884F43DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12528" xr2:uid="{6FE9F777-6649-4D3C-B271-CDD8A66E49D5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{6FE9F777-6649-4D3C-B271-CDD8A66E49D5}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>AreaTooSmall</t>
   </si>
   <si>
-    <t>ValidateGeometry -&gt; TestIfAreaSmallerThan</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Is area at least </t>
     </r>
@@ -214,9 +211,6 @@
     <t>TooSmallVertexCount</t>
   </si>
   <si>
-    <t>ValidateGeometry -&gt; TestIfVertexCounterSmallerThan</t>
-  </si>
-  <si>
     <t>GroundOverlappingIn2D</t>
   </si>
   <si>
@@ -308,15 +302,6 @@
   </si>
   <si>
     <t>ValidateGeometry -&gt; GeometryFilter</t>
-  </si>
-  <si>
-    <t>Is geometry type point, raster, null or point cloud?</t>
-  </si>
-  <si>
-    <t>Geometry type cannot be point, raster, null or point cloud.</t>
-  </si>
-  <si>
-    <t>Geometry type must be valid.</t>
   </si>
   <si>
     <t>Geometry cannot contain NaNs or infinities.</t>
@@ -1134,6 +1119,23 @@
   </si>
   <si>
     <t>This is the GitHub repository, where you can find the updated version of this Excel and the FME quality software.</t>
+  </si>
+  <si>
+    <t>Is geometry type Solid or Surface?</t>
+  </si>
+  <si>
+    <t>Geometry type cannot be anything else than Solid or Surface.</t>
+  </si>
+  <si>
+    <t>Geometry type must be Solid or Surface.</t>
+  </si>
+  <si>
+    <t>ValidateGeometry -&gt;
+CheckMeasurements -&gt; TestIfAreaSmallerThan</t>
+  </si>
+  <si>
+    <t>ValidateGeometry -&gt;
+CheckMeasurements -&gt; TestIfVertexCounterSmallerThan</t>
   </si>
 </sst>
 </file>
@@ -2174,7 +2176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60BBD23-8572-49A2-BECB-70E102A515DD}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2189,7 +2191,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="48" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -2200,7 +2202,7 @@
     </row>
     <row r="2" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -2220,20 +2222,20 @@
     </row>
     <row r="4" spans="1:7" s="47" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
@@ -2242,10 +2244,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C6" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2261,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C7" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2277,7 +2279,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C8" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2293,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C9" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#quality-elements", "Link to wiki page")</f>
@@ -2306,7 +2308,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C10" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2319,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C11" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#implementation-status", "Link to wiki page")</f>
@@ -2332,7 +2334,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C12" s="55" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#error-concequences-severity", "Link to wiki page")</f>
@@ -2344,7 +2346,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C13" s="49"/>
     </row>
@@ -2353,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C14" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#usable-key-words-for-error-messages-and-definitions", "Link to wiki page")</f>
@@ -2365,7 +2367,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C15" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2377,7 +2379,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C16" s="49"/>
     </row>
@@ -2386,7 +2388,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C17" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#version-control", "Link to wiki page")</f>
@@ -2405,17 +2407,17 @@
     </row>
     <row r="21" spans="1:8" s="47" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:8" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C22" s="49"/>
       <c r="D22" s="47" t="str">
@@ -2429,7 +2431,7 @@
         <v>GitHub Wiki</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C23" s="49"/>
     </row>
@@ -2439,7 +2441,7 @@
         <v>GitHub Repository</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C24" s="49"/>
     </row>
@@ -2449,7 +2451,7 @@
         <v>OGC CityGML Standard</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C25" s="49"/>
     </row>
@@ -2459,7 +2461,7 @@
         <v>SIG3D Modelling Guide for 3D Objects: Part 2</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C26" s="49"/>
     </row>
@@ -2469,7 +2471,7 @@
         <v>GeoE3 Project website</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C27" s="49"/>
     </row>
@@ -2493,8 +2495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD580389-2C7D-4A84-8EED-658C64708058}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,7 +2518,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2554,7 +2556,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -2570,34 +2572,34 @@
     </row>
     <row r="3" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K3" s="37"/>
       <c r="L3" s="38">
@@ -2607,31 +2609,31 @@
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="60"/>
       <c r="B4" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K4" s="37"/>
       <c r="L4" s="38">
@@ -2641,34 +2643,34 @@
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="60"/>
       <c r="B5" s="12" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="L5" s="38">
         <v>1</v>
@@ -2677,13 +2679,13 @@
     <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="60"/>
       <c r="B6" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>32</v>
@@ -2692,7 +2694,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H6" s="37" t="s">
         <v>33</v>
@@ -2712,7 +2714,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="59" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -2728,28 +2730,28 @@
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I8" s="37" t="s">
         <v>14</v>
@@ -2758,7 +2760,7 @@
         <v>15</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L8" s="38">
         <v>1</v>
@@ -2767,31 +2769,31 @@
     <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="60"/>
       <c r="B9" s="41" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K9" s="37"/>
       <c r="L9" s="38">
@@ -2801,34 +2803,34 @@
     <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="60"/>
       <c r="B10" s="39" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L10" s="40">
         <v>1</v>
@@ -2836,7 +2838,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -2852,37 +2854,37 @@
     </row>
     <row r="12" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F12" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L12" s="38">
         <v>1</v>
@@ -2891,16 +2893,16 @@
     <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="60"/>
       <c r="B13" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F13" s="37" t="s">
         <v>12</v>
@@ -2918,7 +2920,7 @@
         <v>20</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L13" s="38">
         <v>1</v>
@@ -2927,34 +2929,34 @@
     <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="60"/>
       <c r="B14" s="12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F14" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K14" s="37" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="L14" s="38">
         <v>1</v>
@@ -2963,11 +2965,11 @@
     <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="60"/>
       <c r="B15" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="36" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37" t="s">
@@ -2993,11 +2995,11 @@
     <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="60"/>
       <c r="B16" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="36" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37" t="s">
@@ -3016,7 +3018,7 @@
         <v>27</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="L16" s="38">
         <v>1</v>
@@ -3025,11 +3027,11 @@
     <row r="17" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="60"/>
       <c r="B17" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="36" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37" t="s">
@@ -3054,7 +3056,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="59" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -3070,73 +3072,73 @@
     </row>
     <row r="19" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="60" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F19" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>80</v>
+        <v>309</v>
       </c>
       <c r="I19" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="K19" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="J19" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="K19" s="37" t="s">
-        <v>86</v>
-      </c>
       <c r="L19" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="60"/>
       <c r="B20" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I20" s="37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K20" s="37" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L20" s="38">
         <v>1</v>
@@ -3145,34 +3147,34 @@
     <row r="21" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="60"/>
       <c r="B21" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L21" s="38">
         <v>1</v>
@@ -3181,31 +3183,31 @@
     <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="60"/>
       <c r="B22" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F22" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K22" s="37"/>
       <c r="L22" s="38">
@@ -3215,31 +3217,31 @@
     <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="60"/>
       <c r="B23" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F23" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K23" s="37"/>
       <c r="L23" s="38">
@@ -3249,31 +3251,31 @@
     <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="60"/>
       <c r="B24" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F24" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>41</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="38">
@@ -3283,22 +3285,22 @@
     <row r="25" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="60"/>
       <c r="B25" s="41" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>38</v>
@@ -3310,7 +3312,7 @@
         <v>40</v>
       </c>
       <c r="K25" s="37" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L25" s="38">
         <v>1</v>
@@ -3319,31 +3321,31 @@
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="60"/>
       <c r="B26" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I26" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="K26" s="37"/>
       <c r="L26" s="38">
@@ -3353,16 +3355,16 @@
     <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="60"/>
       <c r="B27" s="41" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>12</v>
@@ -3371,13 +3373,13 @@
         <v>9</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K27" s="37"/>
       <c r="L27" s="38">
@@ -3387,16 +3389,16 @@
     <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="60"/>
       <c r="B28" s="41" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>12</v>
@@ -3405,13 +3407,13 @@
         <v>9</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="K28" s="37"/>
       <c r="L28" s="38">
@@ -3421,16 +3423,16 @@
     <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="60"/>
       <c r="B29" s="41" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>12</v>
@@ -3439,13 +3441,13 @@
         <v>9</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K29" s="37"/>
       <c r="L29" s="38">
@@ -3455,16 +3457,16 @@
     <row r="30" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="60"/>
       <c r="B30" s="41" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>12</v>
@@ -3473,13 +3475,13 @@
         <v>9</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K30" s="37"/>
       <c r="L30" s="38">
@@ -3489,34 +3491,34 @@
     <row r="31" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A31" s="60"/>
       <c r="B31" s="41" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F31" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K31" s="37" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="L31" s="38">
         <v>1</v>
@@ -3525,13 +3527,13 @@
     <row r="32" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="60"/>
       <c r="B32" s="41" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>37</v>
@@ -3543,34 +3545,34 @@
         <v>9</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I32" s="37" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K32" s="37" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="L32" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="60"/>
       <c r="B33" s="41" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>43</v>
+        <v>312</v>
       </c>
       <c r="F33" s="37" t="s">
         <v>12</v>
@@ -3579,47 +3581,47 @@
         <v>9</v>
       </c>
       <c r="H33" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="I33" s="37" t="s">
+      <c r="J33" s="37" t="s">
         <v>45</v>
-      </c>
-      <c r="J33" s="37" t="s">
-        <v>46</v>
       </c>
       <c r="K33" s="37"/>
       <c r="L33" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="60"/>
       <c r="B34" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>48</v>
+        <v>313</v>
       </c>
       <c r="F34" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="H34" s="37" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I34" s="37" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J34" s="37" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="K34" s="37"/>
       <c r="L34" s="38">
@@ -3629,34 +3631,34 @@
     <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" s="60"/>
       <c r="B35" s="41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F35" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H35" s="37" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I35" s="37" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J35" s="37" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K35" s="42" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="L35" s="38">
         <v>1</v>
@@ -3665,16 +3667,16 @@
     <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="60"/>
       <c r="B36" s="41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E36" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F36" s="37" t="s">
         <v>12</v>
@@ -3683,13 +3685,13 @@
         <v>9</v>
       </c>
       <c r="H36" s="37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I36" s="37" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K36" s="37"/>
       <c r="L36" s="38">
@@ -3699,16 +3701,16 @@
     <row r="37" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="60"/>
       <c r="B37" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F37" s="37" t="s">
         <v>12</v>
@@ -3717,13 +3719,13 @@
         <v>9</v>
       </c>
       <c r="H37" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J37" s="37" t="s">
         <v>54</v>
-      </c>
-      <c r="I37" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="J37" s="37" t="s">
-        <v>56</v>
       </c>
       <c r="K37" s="37"/>
       <c r="L37" s="38">
@@ -3733,16 +3735,16 @@
     <row r="38" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="60"/>
       <c r="B38" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F38" s="37" t="s">
         <v>12</v>
@@ -3751,13 +3753,13 @@
         <v>9</v>
       </c>
       <c r="H38" s="37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I38" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J38" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K38" s="37"/>
       <c r="L38" s="38">
@@ -3767,16 +3769,16 @@
     <row r="39" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="60"/>
       <c r="B39" s="41" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F39" s="37" t="s">
         <v>12</v>
@@ -3785,13 +3787,13 @@
         <v>9</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I39" s="37" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J39" s="37" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K39" s="37"/>
       <c r="L39" s="38">
@@ -3801,16 +3803,16 @@
     <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="60"/>
       <c r="B40" s="41" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F40" s="37" t="s">
         <v>12</v>
@@ -3819,13 +3821,13 @@
         <v>9</v>
       </c>
       <c r="H40" s="37" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I40" s="37" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="J40" s="37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K40" s="37"/>
       <c r="L40" s="38">
@@ -3835,16 +3837,16 @@
     <row r="41" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="60"/>
       <c r="B41" s="41" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E41" s="37" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>12</v>
@@ -3853,16 +3855,16 @@
         <v>9</v>
       </c>
       <c r="H41" s="37" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I41" s="37" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J41" s="37" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="K41" s="37" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="L41" s="38">
         <v>1</v>
@@ -3870,7 +3872,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="59" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -3886,19 +3888,19 @@
     </row>
     <row r="43" spans="1:12" s="7" customFormat="1" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="60" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F43" s="37" t="s">
         <v>12</v>
@@ -3907,16 +3909,16 @@
         <v>9</v>
       </c>
       <c r="H43" s="36" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="K43" s="37" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="L43" s="38">
         <v>1</v>
@@ -3925,16 +3927,16 @@
     <row r="44" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="60"/>
       <c r="B44" s="12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>12</v>
@@ -3943,16 +3945,16 @@
         <v>9</v>
       </c>
       <c r="H44" s="36" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I44" s="36" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="J44" s="37" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="K44" s="37" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="L44" s="38">
         <v>1</v>
@@ -3964,13 +3966,13 @@
         <v>31</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E45" s="37" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F45" s="37" t="s">
         <v>12</v>
@@ -3979,16 +3981,16 @@
         <v>9</v>
       </c>
       <c r="H45" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J45" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="I45" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="J45" s="37" t="s">
-        <v>78</v>
-      </c>
       <c r="K45" s="37" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="L45" s="38">
         <v>1</v>
@@ -3996,7 +3998,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="59" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B46" s="59"/>
       <c r="C46" s="43"/>
@@ -4012,32 +4014,32 @@
     </row>
     <row r="47" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="60" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F47" s="37" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G47" s="37" t="s">
         <v>9</v>
       </c>
       <c r="H47" s="36" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J47" s="37" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K47" s="36" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L47" s="40">
         <v>1</v>
@@ -4046,16 +4048,16 @@
     <row r="48" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="60"/>
       <c r="B48" s="39" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F48" s="37" t="s">
         <v>12</v>
@@ -4064,16 +4066,16 @@
         <v>9</v>
       </c>
       <c r="H48" s="37" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I48" s="37" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="J48" s="37" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="L48" s="40">
         <v>1</v>
@@ -4081,7 +4083,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B49" s="44"/>
       <c r="C49" s="43"/>
@@ -4097,19 +4099,19 @@
     </row>
     <row r="50" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="60" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E50" s="45" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F50" s="37" t="s">
         <v>12</v>
@@ -4118,13 +4120,13 @@
         <v>9</v>
       </c>
       <c r="H50" s="37" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I50" s="37" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="J50" s="37" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="K50" s="42"/>
       <c r="L50" s="40">
@@ -4134,16 +4136,16 @@
     <row r="51" spans="1:12" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="60"/>
       <c r="B51" s="39" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E51" s="45" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F51" s="37" t="s">
         <v>12</v>
@@ -4152,13 +4154,13 @@
         <v>9</v>
       </c>
       <c r="H51" s="37" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I51" s="37" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="J51" s="37" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="K51" s="42"/>
       <c r="L51" s="40">
@@ -4313,7 +4315,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4351,7 +4353,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -4367,7 +4369,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="9"/>
@@ -4445,7 +4447,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="61"/>
@@ -4461,7 +4463,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="60" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4554,7 +4556,7 @@
     </row>
     <row r="17" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="61"/>
       <c r="C17" s="61"/>
@@ -4570,7 +4572,7 @@
     </row>
     <row r="18" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="60" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4871,7 +4873,7 @@
     </row>
     <row r="41" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="61" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -4887,7 +4889,7 @@
     </row>
     <row r="42" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="60" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -4973,7 +4975,7 @@
     </row>
     <row r="48" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="61" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B48" s="61"/>
       <c r="C48" s="13"/>
@@ -4989,7 +4991,7 @@
     </row>
     <row r="49" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="60" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -5014,7 +5016,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="30" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="13"/>
@@ -5030,7 +5032,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="60" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>

</xml_diff>

<commit_message>
Updated CityGML versions. Added CityJSON versions.
Both are still beta version without proper testing.
</commit_message>
<xml_diff>
--- a/QualityRules_CityGML.xlsx
+++ b/QualityRules_CityGML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATURUNEN\Work Folders\FME+DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F11225-C68A-403C-B267-941884F43DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECE5307-6C5C-43E0-9878-CCD0202F7183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{6FE9F777-6649-4D3C-B271-CDD8A66E49D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12528" activeTab="1" xr2:uid="{6FE9F777-6649-4D3C-B271-CDD8A66E49D5}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="317">
   <si>
     <t>QUALITY ELEMENT</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">Attribute information XXX must have value based on data model. </t>
-  </si>
-  <si>
-    <t>Is the value between A…N?</t>
   </si>
   <si>
     <t>The value of the attribute XXX is not in allowed range (A-N)? </t>
@@ -148,18 +145,6 @@
     <t>GML Reader fix that automatically</t>
   </si>
   <si>
-    <t>Is the end point of the feature same as start point?</t>
-  </si>
-  <si>
-    <t>End point is not same as start point.</t>
-  </si>
-  <si>
-    <t>Feature must be self-closure based on its starting and ending points.</t>
-  </si>
-  <si>
-    <t>Because GML Reader will fix this automatically, the error is not included to the quality report</t>
-  </si>
-  <si>
     <t>GeometryValidator -&gt; CheckOGCSimple</t>
   </si>
   <si>
@@ -178,45 +163,9 @@
     <t>AreaTooSmall</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Is area at least </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> m²?</t>
-    </r>
-  </si>
-  <si>
-    <t>The area of the geometry is not 1 m² at minimum.</t>
-  </si>
-  <si>
-    <t>The area of the geometry must be at least 1 m².</t>
-  </si>
-  <si>
-    <t>TooSmallVertexCount</t>
-  </si>
-  <si>
     <t>GroundOverlappingIn2D</t>
   </si>
   <si>
-    <t xml:space="preserve">Is GroundSurface overlapping with GroundSurface of another Building? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Overlapping area of two features must be smaller than 5 % of their areas. </t>
   </si>
   <si>
@@ -226,9 +175,6 @@
     <t>CompareRoofToFloor</t>
   </si>
   <si>
-    <t>Is minimum height of the roof higher than minimum height of the floor?</t>
-  </si>
-  <si>
     <t>The minimum height of the roof cannot be smaller than minimum height of the ground.</t>
   </si>
   <si>
@@ -250,9 +196,6 @@
     <t>FindDuplicateGeometries</t>
   </si>
   <si>
-    <t>Is geometry unique for all features?</t>
-  </si>
-  <si>
     <t>Geometry must be unique for all features</t>
   </si>
   <si>
@@ -274,9 +217,6 @@
     <t>DuplicateIDFilter</t>
   </si>
   <si>
-    <t>Is ID unique for all features during the execution?</t>
-  </si>
-  <si>
     <t>DuplicateID</t>
   </si>
   <si>
@@ -304,42 +244,15 @@
     <t>ValidateGeometry -&gt; GeometryFilter</t>
   </si>
   <si>
-    <t>Geometry cannot contain NaNs or infinities.</t>
-  </si>
-  <si>
-    <t>Does geometry contain NaNs or infinities?</t>
-  </si>
-  <si>
-    <t>Geometry must be valid.</t>
-  </si>
-  <si>
     <t>Failed features are discarded because otherwise they would affect to other rules</t>
   </si>
   <si>
-    <t>Does geometrycontain degenerated or corrupted geometries?</t>
-  </si>
-  <si>
-    <t>Geometry cannot contain degenerated or corrupted geometries.</t>
-  </si>
-  <si>
     <t>NonPlanarByNormals</t>
   </si>
   <si>
     <t>NonPlanarByThickness</t>
   </si>
   <si>
-    <t>Is face or boundary surface planar based on normal deviation?</t>
-  </si>
-  <si>
-    <t>Is face or boundary surface planar based on thickness?</t>
-  </si>
-  <si>
-    <t>Face or boundary surface cannot be non-planar.</t>
-  </si>
-  <si>
-    <t>Face or boundary surface must be planar.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 	Contains NaNs or Infinities</t>
   </si>
   <si>
@@ -388,12 +301,6 @@
     <t xml:space="preserve">Geometries must be either 2D or 3D, not both. </t>
   </si>
   <si>
-    <t>The feature has not vertex normals.</t>
-  </si>
-  <si>
-    <t>Does the feature have vertex normals?</t>
-  </si>
-  <si>
     <t>Does the feature have a mixture of 2D and 3D parts?</t>
   </si>
   <si>
@@ -412,13 +319,7 @@
     <t>The surface cannot have an incorrect orientation.</t>
   </si>
   <si>
-    <t>The area cannot have an incorret orientation.</t>
-  </si>
-  <si>
     <t>The area must have a valid orientation.</t>
-  </si>
-  <si>
-    <t>Does all others vertices have values for either a measure or the elevations, if at least one vertice has a value.</t>
   </si>
   <si>
     <t>The feature does not contain values for the elevation or a measure.</t>
@@ -509,9 +410,6 @@
 -Invalid Solid Boundaries</t>
   </si>
   <si>
-    <t>The solid cannot be invalid.</t>
-  </si>
-  <si>
     <t>The solid must be valid.</t>
   </si>
   <si>
@@ -545,18 +443,9 @@
     <t>CheckCRS -&gt; Check3D</t>
   </si>
   <si>
-    <t>Is coordinate reference system 3D?</t>
-  </si>
-  <si>
     <t>Does every building/buildingpart has a coordinate reference system?</t>
   </si>
   <si>
-    <t>Coordinate reference system is not 3d</t>
-  </si>
-  <si>
-    <t>Coordinate reference system must be 3d</t>
-  </si>
-  <si>
     <t>MissingAddressInformation</t>
   </si>
   <si>
@@ -567,9 +456,6 @@
   </si>
   <si>
     <t>The address feature must contain all needed information</t>
-  </si>
-  <si>
-    <t>Does address feature has information about Country, Locality, PostalCode, ThoroughfareNumber and ThoroughfareName?</t>
   </si>
   <si>
     <t>The address feature does not contain all needed information.</t>
@@ -594,12 +480,6 @@
     <t>Conceptual Consistenxy</t>
   </si>
   <si>
-    <t>Does solid have an correct orientation?</t>
-  </si>
-  <si>
-    <t>Does surface have an correct orientation?</t>
-  </si>
-  <si>
     <t>Does Areas, such as polygons, ellipses, and donuts, have an correct orientation?</t>
   </si>
   <si>
@@ -621,9 +501,6 @@
     <t>ValidateXlinks</t>
   </si>
   <si>
-    <t>Does LoD2 Solid contain SurfaceMembers without linked xlinks?</t>
-  </si>
-  <si>
     <t>Conceptual Consistency</t>
   </si>
   <si>
@@ -655,9 +532,6 @@
   </si>
   <si>
     <t>Does every address feature correspond to external address information system?</t>
-  </si>
-  <si>
-    <t>Address not found in external address information system.</t>
   </si>
   <si>
     <t>Every address feature must be found on external address information system.</t>
@@ -724,18 +598,9 @@
     <t>CheckFmeType</t>
   </si>
   <si>
-    <t>Does feature has fme_type defined?</t>
-  </si>
-  <si>
-    <t>All features must have fme_type</t>
-  </si>
-  <si>
     <t>MissingFmeType</t>
   </si>
   <si>
-    <t>The feature does not have fme_type ie. it contain no points.</t>
-  </si>
-  <si>
     <t>These rules process xlinks of the data.</t>
   </si>
   <si>
@@ -745,15 +610,6 @@
     <t>ValidateAttributes checks that attribute fields and values are logical and follows the recommendation</t>
   </si>
   <si>
-    <t>Does geometry contain at least 4 vertices?</t>
-  </si>
-  <si>
-    <t>The number of vertices in geometry must be greater than 3</t>
-  </si>
-  <si>
-    <t>The number of vertices in geometry cannot be smaller than 4</t>
-  </si>
-  <si>
     <t>ValidateGeometry -&gt; CheckAndFixNonPlanarity</t>
   </si>
   <si>
@@ -770,9 +626,6 @@
   </si>
   <si>
     <t>ValidateGeometry -&gt; CheckNormals</t>
-  </si>
-  <si>
-    <t>Normal of the face is not logically oriented.</t>
   </si>
   <si>
     <t>All normals of the faces must be logically oriented.</t>
@@ -783,13 +636,7 @@
 Z-normals of the WallSurfacez must be between -0.1 and 0.1 to be mostly vertical.</t>
   </si>
   <si>
-    <t>Is every face of the feature logically oriented based on vertex normals and depending on the feature type?</t>
-  </si>
-  <si>
     <t>CheckHierarcy</t>
-  </si>
-  <si>
-    <t>Does every feature (Address feature or Roof-, Ground-, or WallSurface) match with some Building or BuildingPart?</t>
   </si>
   <si>
     <t>The feature XXX can not be assigned to any Building or BuildingPart.</t>
@@ -813,9 +660,6 @@
     <t xml:space="preserve">CheckHierarcy </t>
   </si>
   <si>
-    <t>Does every Building or BuildingPart has all needed features (Address feature) and surfaces (Roof-, Ground- and WallSurface)?</t>
-  </si>
-  <si>
     <t>Building or BuildingPart has no XXX feature.</t>
   </si>
   <si>
@@ -828,19 +672,10 @@
     <t>MissingXLink</t>
   </si>
   <si>
-    <t>SurfaceMember must be linked to some Building or BuildingPart with xlinks.</t>
-  </si>
-  <si>
     <t>All SurfaceMembers of LoD2-Solid must be linked with xlinks.</t>
   </si>
   <si>
     <t>Is every SurfaceMember linked to at least one Building or Buildingpart with xlinks?</t>
-  </si>
-  <si>
-    <t>SurfaceMember is not correctly linked to Building or BuildingPart with xlinks.</t>
-  </si>
-  <si>
-    <t>Lod2 Solid cannot contain SurfaceMembers without linked xlink.</t>
   </si>
   <si>
     <t>CheckCRS -&gt; GeometryValidator</t>
@@ -1046,9 +881,6 @@
     <t>ValidateGeometry15</t>
   </si>
   <si>
-    <t>ValidateGeometry16</t>
-  </si>
-  <si>
     <t>ValidateGeometry17</t>
   </si>
   <si>
@@ -1121,21 +953,179 @@
     <t>This is the GitHub repository, where you can find the updated version of this Excel and the FME quality software.</t>
   </si>
   <si>
-    <t>Is geometry type Solid or Surface?</t>
-  </si>
-  <si>
-    <t>Geometry type cannot be anything else than Solid or Surface.</t>
-  </si>
-  <si>
-    <t>Geometry type must be Solid or Surface.</t>
-  </si>
-  <si>
     <t>ValidateGeometry -&gt;
 CheckMeasurements -&gt; TestIfAreaSmallerThan</t>
   </si>
   <si>
+    <t>Is the geometry unique for all features?</t>
+  </si>
+  <si>
+    <t>Is the ID unique for all features?</t>
+  </si>
+  <si>
+    <t>Does the feature has geometry?</t>
+  </si>
+  <si>
+    <t>The feature does not contain points.</t>
+  </si>
+  <si>
+    <t>All features must contain points ie. fme_tpe cannot be missing.</t>
+  </si>
+  <si>
+    <t>Is the end point of the feature same as the start point?</t>
+  </si>
+  <si>
+    <t>The feature must be self-closure based on its starting and ending points.</t>
+  </si>
+  <si>
+    <t>The feature is not self-closure.</t>
+  </si>
+  <si>
+    <t>Because GML Reader fix this automatically, the error is not included to the quality report.</t>
+  </si>
+  <si>
+    <t>Is the coordinate reference system 3D?</t>
+  </si>
+  <si>
+    <t>The coordinate reference system is not 3d</t>
+  </si>
+  <si>
+    <t>The coordinate reference system must be 3d</t>
+  </si>
+  <si>
+    <t>Is the geometry type Solid or Surface?</t>
+  </si>
+  <si>
+    <t>The geometry type cannot be anything else than Solid or Surface.</t>
+  </si>
+  <si>
+    <t>The geometry type must be Solid or Surface.</t>
+  </si>
+  <si>
+    <t>Does the geometry contain NaNs or infinities?</t>
+  </si>
+  <si>
+    <t>The geometry cannot contain NaNs or infinities.</t>
+  </si>
+  <si>
+    <t>Does the geometry contain degenerated or corrupted geometries?</t>
+  </si>
+  <si>
+    <t>The geometry cannot contain degenerated or corrupted geometries.</t>
+  </si>
+  <si>
+    <t>The geometry must be valid.</t>
+  </si>
+  <si>
+    <t>Is the Face or BoundarySurface planar based on normal deviation?</t>
+  </si>
+  <si>
+    <t>Face or BoundarySurface cannot be curved.</t>
+  </si>
+  <si>
+    <t>Is the Face or BoundarySurface planar based on thickness?</t>
+  </si>
+  <si>
+    <t>The face or BoundarySurface must be planar.</t>
+  </si>
+  <si>
+    <t>The Face or BoundarySurface must be planar.</t>
+  </si>
+  <si>
+    <t>Does the feature has vertex normals?</t>
+  </si>
+  <si>
+    <t>The feature has no vertex normals.</t>
+  </si>
+  <si>
+    <t>Does the surface has an correct orientation?</t>
+  </si>
+  <si>
+    <t>Does the solid has an correct orientation?</t>
+  </si>
+  <si>
+    <t>The area cannot have an incorrect orientation.</t>
+  </si>
+  <si>
+    <t>Does the all others vertices have values for either a measure or the elevations, if at least one vertice has a value.</t>
+  </si>
+  <si>
+    <t>Is the area at least X m²?</t>
+  </si>
+  <si>
+    <t>The area of the geometry is not X m² at minimum.</t>
+  </si>
+  <si>
+    <t>The area of the geometry must be at least X m².</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum area can be defined from user parameters.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum number of vertices can be defined from user parameters.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the GroundSurface overlapping with the GroundSurface of another Building? </t>
+  </si>
+  <si>
+    <t>Is the minimum height of the roof higher than minimum height of the floor?</t>
+  </si>
+  <si>
+    <t>The solid cannot contain problems.</t>
+  </si>
+  <si>
+    <t>Is the every face of the feature logically oriented based on vertex normals and depending on the feature type?</t>
+  </si>
+  <si>
+    <t>The normal of the face is not logically oriented.</t>
+  </si>
+  <si>
+    <t>Does the every Building or BuildingPart has all needed features (Address feature) and surfaces (Roof-, Ground- and WallSurface)?</t>
+  </si>
+  <si>
+    <t>Does the every feature (Address feature or Roof-, Ground-, or WallSurface) match with some Building or BuildingPart?</t>
+  </si>
+  <si>
+    <t>Does the address feature has information about Country, Locality, PostalCode, ThoroughfareNumber and ThoroughfareName?</t>
+  </si>
+  <si>
+    <t>The address not found in external address information system.</t>
+  </si>
+  <si>
+    <t>Does the LoD2 Solid contain SurfaceMembers without linked xlinks?</t>
+  </si>
+  <si>
+    <t>The lod2 Solid cannot contain SurfaceMembers without linked xlink.</t>
+  </si>
+  <si>
+    <t>The SurfaceMember is not correctly linked to Building or BuildingPart with xlinks.</t>
+  </si>
+  <si>
+    <t>The SurfaceMember must be linked to some Building or BuildingPart with xlinks.</t>
+  </si>
+  <si>
+    <t>Is the value in the range A…N?</t>
+  </si>
+  <si>
+    <t>TooSmallVolume</t>
+  </si>
+  <si>
     <t>ValidateGeometry -&gt;
-CheckMeasurements -&gt; TestIfVertexCounterSmallerThan</t>
+CheckMeasurements -&gt; TestIfVolumeSmallerThan</t>
+  </si>
+  <si>
+    <t>Is the volume of the solid at least X m3?</t>
+  </si>
+  <si>
+    <t>The volume of the solid cannot be smaller than X m3.</t>
+  </si>
+  <si>
+    <t>The volume of the solid must be greater than X m3..</t>
+  </si>
+  <si>
+    <t>ValidateGeometry24</t>
   </si>
 </sst>
 </file>
@@ -1504,11 +1494,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1521,7 +1511,7 @@
     <cellStyle name="Normaali 2" xfId="3" xr:uid="{7E3974D2-0DBE-4F5E-9E3D-6576F2D20CDD}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="48">
     <dxf>
       <font>
         <b/>
@@ -1624,6 +1614,75 @@
         <b/>
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -1853,12 +1912,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F47F029-A215-4390-BD70-0FA320C2B170}" name="Table2" displayName="Table2" ref="A5:C17" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" headerRowCellStyle="Normaali 2" dataCellStyle="Normaali 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F47F029-A215-4390-BD70-0FA320C2B170}" name="Table2" displayName="Table2" ref="A5:C17" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowCellStyle="Normaali 2" dataCellStyle="Normaali 2">
   <autoFilter ref="A5:C17" xr:uid="{C38A5F96-A0AA-4876-B4C5-E49F96B5CEDA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6F199324-BC17-4B16-8679-AB40CD4CC31A}" name="Excel Column Name" dataDxfId="35" dataCellStyle="Normaali 2"/>
-    <tableColumn id="2" xr3:uid="{3560AFFA-3F2B-4245-9538-C1649867110F}" name="Column Description" dataDxfId="34" dataCellStyle="Normaali 2"/>
-    <tableColumn id="3" xr3:uid="{95B4044B-30D4-47CE-AE75-E6B0AB8A1CDE}" name="More info" dataDxfId="33" dataCellStyle="Normaali 2">
+    <tableColumn id="1" xr3:uid="{6F199324-BC17-4B16-8679-AB40CD4CC31A}" name="Excel Column Name" dataDxfId="45" dataCellStyle="Normaali 2"/>
+    <tableColumn id="2" xr3:uid="{3560AFFA-3F2B-4245-9538-C1649867110F}" name="Column Description" dataDxfId="44" dataCellStyle="Normaali 2"/>
+    <tableColumn id="3" xr3:uid="{95B4044B-30D4-47CE-AE75-E6B0AB8A1CDE}" name="More info" dataDxfId="43" dataCellStyle="Normaali 2">
       <calculatedColumnFormula>HYPERLINK("")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1867,11 +1926,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8C90D32-6635-456E-8479-2F97FE9D02D7}" name="Table24" displayName="Table24" ref="A22:B27" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowCellStyle="Normaali 2" dataCellStyle="Normaali 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8C90D32-6635-456E-8479-2F97FE9D02D7}" name="Table24" displayName="Table24" ref="A22:B27" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" headerRowCellStyle="Normaali 2" dataCellStyle="Normaali 2">
   <autoFilter ref="A22:B27" xr:uid="{E861418B-8CA0-4956-8281-E50B007FE59E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DF37DB37-B34B-4CFD-82AF-66DCB0433FA6}" name="Link" dataDxfId="30" dataCellStyle="Normaali 2"/>
-    <tableColumn id="2" xr3:uid="{96312410-A187-46F8-BAA1-0EAE24590084}" name="Link Description" dataDxfId="29" dataCellStyle="Normaali 2"/>
+    <tableColumn id="1" xr3:uid="{DF37DB37-B34B-4CFD-82AF-66DCB0433FA6}" name="Link" dataDxfId="40" dataCellStyle="Normaali 2"/>
+    <tableColumn id="2" xr3:uid="{96312410-A187-46F8-BAA1-0EAE24590084}" name="Link Description" dataDxfId="39" dataCellStyle="Normaali 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2191,7 +2250,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="48" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -2202,7 +2261,7 @@
     </row>
     <row r="2" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>307</v>
+        <v>258</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -2222,20 +2281,20 @@
     </row>
     <row r="4" spans="1:7" s="47" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
@@ -2244,10 +2303,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C6" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2263,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>305</v>
+        <v>256</v>
       </c>
       <c r="C7" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2279,7 +2338,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>306</v>
+        <v>257</v>
       </c>
       <c r="C8" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2295,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>260</v>
+        <v>212</v>
       </c>
       <c r="C9" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#quality-elements", "Link to wiki page")</f>
@@ -2308,7 +2367,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
       <c r="C10" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2321,7 +2380,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
       <c r="C11" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#implementation-status", "Link to wiki page")</f>
@@ -2334,7 +2393,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="C12" s="55" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#error-concequences-severity", "Link to wiki page")</f>
@@ -2346,7 +2405,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="C13" s="49"/>
     </row>
@@ -2355,7 +2414,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="C14" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#usable-key-words-for-error-messages-and-definitions", "Link to wiki page")</f>
@@ -2367,7 +2426,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="C15" s="49" t="str">
         <f>HYPERLINK("")</f>
@@ -2379,7 +2438,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
       <c r="C16" s="49"/>
     </row>
@@ -2388,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="C17" s="49" t="str">
         <f>HYPERLINK("https://github.com/opengeospatial/GEOE3/wiki/Quality_Rules#version-control", "Link to wiki page")</f>
@@ -2407,17 +2466,17 @@
     </row>
     <row r="21" spans="1:8" s="47" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>247</v>
+        <v>199</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:8" s="47" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="C22" s="49"/>
       <c r="D22" s="47" t="str">
@@ -2431,7 +2490,7 @@
         <v>GitHub Wiki</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="C23" s="49"/>
     </row>
@@ -2441,7 +2500,7 @@
         <v>GitHub Repository</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>308</v>
+        <v>259</v>
       </c>
       <c r="C24" s="49"/>
     </row>
@@ -2451,7 +2510,7 @@
         <v>OGC CityGML Standard</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="C25" s="49"/>
     </row>
@@ -2461,7 +2520,7 @@
         <v>SIG3D Modelling Guide for 3D Objects: Part 2</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="C26" s="49"/>
     </row>
@@ -2471,7 +2530,7 @@
         <v>GeoE3 Project website</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="C27" s="49"/>
     </row>
@@ -2495,8 +2554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD580389-2C7D-4A84-8EED-658C64708058}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2518,7 +2577,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2555,51 +2614,51 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="A2" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
       <c r="K2" s="33"/>
       <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60" t="s">
-        <v>168</v>
+      <c r="A3" s="59" t="s">
+        <v>135</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>60</v>
+        <v>261</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="K3" s="37"/>
       <c r="L3" s="38">
@@ -2607,33 +2666,33 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="12" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>262</v>
+        <v>214</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>68</v>
+        <v>262</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="K4" s="37"/>
       <c r="L4" s="38">
@@ -2641,117 +2700,117 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="12" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>208</v>
+        <v>263</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>211</v>
+        <v>264</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>304</v>
+        <v>255</v>
       </c>
       <c r="L5" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="12" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>264</v>
+        <v>216</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>34</v>
+        <v>268</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>35</v>
+        <v>267</v>
       </c>
       <c r="K6" s="37" t="s">
-        <v>36</v>
+        <v>269</v>
       </c>
       <c r="L6" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="A7" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
       <c r="K7" s="33"/>
       <c r="L7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="60" t="s">
-        <v>220</v>
+      <c r="A8" s="59" t="s">
+        <v>179</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="I8" s="37" t="s">
         <v>14</v>
@@ -2760,40 +2819,40 @@
         <v>15</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="L8" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="60"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="41" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>266</v>
+        <v>218</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="K9" s="37"/>
       <c r="L9" s="38">
@@ -2801,108 +2860,108 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="39" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>149</v>
+        <v>270</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>151</v>
+        <v>271</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="L10" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
+      <c r="A11" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
       <c r="K11" s="33"/>
       <c r="L11" s="34"/>
     </row>
     <row r="12" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="60" t="s">
-        <v>214</v>
+      <c r="A12" s="59" t="s">
+        <v>176</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>268</v>
+        <v>220</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
       <c r="F12" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>251</v>
+        <v>203</v>
       </c>
       <c r="L12" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>269</v>
+        <v>221</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
       <c r="F13" s="37" t="s">
         <v>12</v>
@@ -2911,81 +2970,81 @@
         <v>9</v>
       </c>
       <c r="H13" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="I13" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="J13" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="37" t="s">
-        <v>20</v>
-      </c>
       <c r="K13" s="37" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="L13" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="60"/>
+    <row r="14" spans="1:12" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="59"/>
       <c r="B14" s="12" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
       <c r="F14" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="H14" s="37" t="s">
-        <v>177</v>
-      </c>
       <c r="I14" s="37" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="K14" s="37" t="s">
-        <v>252</v>
+        <v>204</v>
       </c>
       <c r="L14" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="12" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="36" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="37" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="37" t="s">
+      <c r="J15" s="37" t="s">
         <v>22</v>
-      </c>
-      <c r="J15" s="37" t="s">
-        <v>23</v>
       </c>
       <c r="K15" s="37"/>
       <c r="L15" s="38">
@@ -2993,61 +3052,61 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="60"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="36" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="J16" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="37" t="s">
-        <v>27</v>
-      </c>
       <c r="K16" s="37" t="s">
-        <v>303</v>
+        <v>254</v>
       </c>
       <c r="L16" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="36" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="37" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="37" t="s">
+      <c r="J17" s="37" t="s">
         <v>29</v>
-      </c>
-      <c r="J17" s="37" t="s">
-        <v>30</v>
       </c>
       <c r="K17" s="37"/>
       <c r="L17" s="38">
@@ -3055,159 +3114,159 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="59" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
+      <c r="A18" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
       <c r="K18" s="33"/>
       <c r="L18" s="34"/>
     </row>
-    <row r="19" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="60" t="s">
-        <v>169</v>
+    <row r="19" spans="1:12" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="59" t="s">
+        <v>136</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>271</v>
+        <v>223</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F19" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
       <c r="I19" s="37" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="K19" s="37" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="L19" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="60"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="12" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>272</v>
+        <v>224</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>79</v>
+        <v>276</v>
       </c>
       <c r="I20" s="37" t="s">
-        <v>78</v>
+        <v>277</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="K20" s="37" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="L20" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="60"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="12" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>273</v>
+        <v>225</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>82</v>
+        <v>278</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>83</v>
+        <v>279</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="L21" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="60"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="12" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>274</v>
+        <v>226</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="F22" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>86</v>
+        <v>281</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>88</v>
+        <v>282</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>89</v>
+        <v>285</v>
       </c>
       <c r="K22" s="37"/>
       <c r="L22" s="38">
@@ -3215,33 +3274,33 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="60"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="12" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="F23" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>87</v>
+        <v>283</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>88</v>
+        <v>282</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>89</v>
+        <v>284</v>
       </c>
       <c r="K23" s="37"/>
       <c r="L23" s="38">
@@ -3249,33 +3308,33 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="60"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="12" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>276</v>
+        <v>228</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="F24" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="38">
@@ -3283,69 +3342,69 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="41" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>277</v>
+        <v>229</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K25" s="37" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="L25" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="41" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>107</v>
+        <v>286</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>106</v>
+        <v>287</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="K26" s="37"/>
       <c r="L26" s="38">
@@ -3353,18 +3412,18 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="60"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="41" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>279</v>
+        <v>231</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>12</v>
@@ -3373,13 +3432,13 @@
         <v>9</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>166</v>
+        <v>288</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="K27" s="37"/>
       <c r="L27" s="38">
@@ -3387,18 +3446,18 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="60"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="41" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>280</v>
+        <v>232</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>12</v>
@@ -3407,13 +3466,13 @@
         <v>9</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>165</v>
+        <v>289</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="K28" s="37"/>
       <c r="L28" s="38">
@@ -3421,18 +3480,18 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="60"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="41" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>281</v>
+        <v>233</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>12</v>
@@ -3441,32 +3500,32 @@
         <v>9</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>114</v>
+        <v>290</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="K29" s="37"/>
       <c r="L29" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
+    <row r="30" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="59"/>
       <c r="B30" s="41" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>282</v>
+        <v>234</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>12</v>
@@ -3475,68 +3534,68 @@
         <v>9</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>116</v>
+        <v>291</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="K30" s="37"/>
       <c r="L30" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="60"/>
+    <row r="31" spans="1:12" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="59"/>
       <c r="B31" s="41" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>283</v>
+        <v>235</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F31" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="K31" s="37" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
       <c r="L31" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="60"/>
+    <row r="32" spans="1:12" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="59"/>
       <c r="B32" s="41" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>284</v>
+        <v>236</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F32" s="37" t="s">
         <v>12</v>
@@ -3545,34 +3604,34 @@
         <v>9</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="I32" s="37" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="K32" s="37" t="s">
-        <v>302</v>
+        <v>253</v>
       </c>
       <c r="L32" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="60"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="41" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>312</v>
+        <v>260</v>
       </c>
       <c r="F33" s="37" t="s">
         <v>12</v>
@@ -3581,102 +3640,104 @@
         <v>9</v>
       </c>
       <c r="H33" s="37" t="s">
-        <v>43</v>
+        <v>292</v>
       </c>
       <c r="I33" s="37" t="s">
-        <v>44</v>
+        <v>293</v>
       </c>
       <c r="J33" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="K33" s="37"/>
+        <v>294</v>
+      </c>
+      <c r="K33" s="37" t="s">
+        <v>295</v>
+      </c>
       <c r="L33" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="60"/>
+    <row r="34" spans="1:12" ht="153" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="59"/>
       <c r="B34" s="41" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>286</v>
+        <v>238</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>313</v>
+        <v>104</v>
       </c>
       <c r="F34" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>9</v>
+        <v>201</v>
       </c>
       <c r="H34" s="37" t="s">
-        <v>215</v>
+        <v>105</v>
       </c>
       <c r="I34" s="37" t="s">
-        <v>217</v>
+        <v>106</v>
       </c>
       <c r="J34" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="K34" s="37"/>
+        <v>107</v>
+      </c>
+      <c r="K34" s="42" t="s">
+        <v>251</v>
+      </c>
       <c r="L34" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A35" s="60"/>
+    <row r="35" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="59"/>
       <c r="B35" s="41" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>287</v>
+        <v>239</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="F35" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>249</v>
+        <v>9</v>
       </c>
       <c r="H35" s="37" t="s">
-        <v>131</v>
+        <v>297</v>
       </c>
       <c r="I35" s="37" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="J35" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="K35" s="42" t="s">
-        <v>300</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="K35" s="37"/>
       <c r="L35" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="60"/>
-      <c r="B36" s="41" t="s">
-        <v>47</v>
+      <c r="A36" s="59"/>
+      <c r="B36" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>288</v>
+        <v>240</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="37" t="s">
-        <v>47</v>
+        <v>141</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="F36" s="37" t="s">
         <v>12</v>
@@ -3685,13 +3746,13 @@
         <v>9</v>
       </c>
       <c r="H36" s="37" t="s">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="I36" s="37" t="s">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K36" s="37"/>
       <c r="L36" s="38">
@@ -3699,18 +3760,18 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="60"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F37" s="37" t="s">
         <v>12</v>
@@ -3719,32 +3780,32 @@
         <v>9</v>
       </c>
       <c r="H37" s="37" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I37" s="37" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J37" s="37" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="K37" s="37"/>
       <c r="L37" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="60"/>
-      <c r="B38" s="12" t="s">
-        <v>55</v>
+    <row r="38" spans="1:12" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="59"/>
+      <c r="B38" s="41" t="s">
+        <v>108</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>51</v>
+        <v>141</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>109</v>
       </c>
       <c r="F38" s="37" t="s">
         <v>12</v>
@@ -3753,32 +3814,32 @@
         <v>9</v>
       </c>
       <c r="H38" s="37" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="I38" s="37" t="s">
-        <v>57</v>
+        <v>299</v>
       </c>
       <c r="J38" s="37" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="K38" s="37"/>
       <c r="L38" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
+    <row r="39" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="59"/>
       <c r="B39" s="41" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="F39" s="37" t="s">
         <v>12</v>
@@ -3787,32 +3848,32 @@
         <v>9</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="I39" s="37" t="s">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="J39" s="37" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="K39" s="37"/>
       <c r="L39" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="60"/>
+    <row r="40" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="59"/>
       <c r="B40" s="41" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F40" s="37" t="s">
         <v>12</v>
@@ -3821,32 +3882,33 @@
         <v>9</v>
       </c>
       <c r="H40" s="37" t="s">
-        <v>192</v>
+        <v>300</v>
       </c>
       <c r="I40" s="37" t="s">
-        <v>246</v>
+        <v>301</v>
       </c>
       <c r="J40" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="K40" s="37"/>
+        <v>183</v>
+      </c>
+      <c r="K40" s="37" t="s">
+        <v>184</v>
+      </c>
       <c r="L40" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="60"/>
+    <row r="41" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B41" s="41" t="s">
-        <v>222</v>
+        <v>311</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="E41" s="37" t="s">
-        <v>223</v>
+        <v>312</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>12</v>
@@ -3855,52 +3917,54 @@
         <v>9</v>
       </c>
       <c r="H41" s="37" t="s">
-        <v>227</v>
+        <v>313</v>
       </c>
       <c r="I41" s="37" t="s">
-        <v>224</v>
+        <v>314</v>
       </c>
       <c r="J41" s="37" t="s">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="K41" s="37" t="s">
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="L41" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
+    <row r="42" spans="1:12" s="7" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
       <c r="K42" s="33"/>
-      <c r="L42" s="34"/>
-    </row>
-    <row r="43" spans="1:12" s="7" customFormat="1" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="60" t="s">
-        <v>170</v>
+      <c r="L42" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="59" t="s">
+        <v>137</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="F43" s="37" t="s">
         <v>12</v>
@@ -3909,34 +3973,34 @@
         <v>9</v>
       </c>
       <c r="H43" s="36" t="s">
-        <v>229</v>
+        <v>303</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
       <c r="K43" s="37" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="L43" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="60"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="12" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>295</v>
+        <v>246</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>12</v>
@@ -3945,34 +4009,34 @@
         <v>9</v>
       </c>
       <c r="H44" s="36" t="s">
-        <v>235</v>
+        <v>302</v>
       </c>
       <c r="I44" s="36" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="J44" s="37" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="K44" s="37" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="L44" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="60"/>
+    <row r="45" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="59"/>
       <c r="B45" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>296</v>
+        <v>247</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E45" s="37" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="F45" s="37" t="s">
         <v>12</v>
@@ -3981,26 +4045,24 @@
         <v>9</v>
       </c>
       <c r="H45" s="36" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I45" s="36" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="J45" s="37" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="K45" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="L45" s="38">
-        <v>1</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="L45" s="34"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="59" t="s">
-        <v>154</v>
-      </c>
-      <c r="B46" s="59"/>
+      <c r="A46" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="60"/>
       <c r="C46" s="43"/>
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
@@ -4010,54 +4072,56 @@
       <c r="I46" s="33"/>
       <c r="J46" s="33"/>
       <c r="K46" s="33"/>
-      <c r="L46" s="34"/>
+      <c r="L46" s="40">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="60" t="s">
-        <v>213</v>
+      <c r="A47" s="59" t="s">
+        <v>175</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="6" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="F47" s="37" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="G47" s="37" t="s">
         <v>9</v>
       </c>
       <c r="H47" s="36" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>186</v>
+        <v>305</v>
       </c>
       <c r="J47" s="37" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="K47" s="36" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="L47" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="60"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="39" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="F48" s="37" t="s">
         <v>12</v>
@@ -4066,24 +4130,22 @@
         <v>9</v>
       </c>
       <c r="H48" s="37" t="s">
-        <v>157</v>
+        <v>304</v>
       </c>
       <c r="I48" s="37" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="J48" s="37" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="L48" s="40">
-        <v>1</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="L48" s="34"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="B49" s="44"/>
       <c r="C49" s="43"/>
@@ -4095,23 +4157,25 @@
       <c r="I49" s="33"/>
       <c r="J49" s="33"/>
       <c r="K49" s="33"/>
-      <c r="L49" s="34"/>
-    </row>
-    <row r="50" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="60" t="s">
-        <v>248</v>
+      <c r="L49" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="59" t="s">
+        <v>200</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>298</v>
+        <v>249</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E50" s="45" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="F50" s="37" t="s">
         <v>12</v>
@@ -4120,32 +4184,32 @@
         <v>9</v>
       </c>
       <c r="H50" s="37" t="s">
-        <v>174</v>
+        <v>306</v>
       </c>
       <c r="I50" s="37" t="s">
-        <v>244</v>
+        <v>307</v>
       </c>
       <c r="J50" s="37" t="s">
-        <v>241</v>
+        <v>195</v>
       </c>
       <c r="K50" s="42"/>
       <c r="L50" s="40">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="60"/>
+    <row r="51" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="59"/>
       <c r="B51" s="39" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>299</v>
+        <v>250</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E51" s="45" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="F51" s="37" t="s">
         <v>12</v>
@@ -4154,30 +4218,27 @@
         <v>9</v>
       </c>
       <c r="H51" s="37" t="s">
-        <v>242</v>
+        <v>196</v>
       </c>
       <c r="I51" s="37" t="s">
-        <v>243</v>
+        <v>308</v>
       </c>
       <c r="J51" s="37" t="s">
-        <v>240</v>
+        <v>309</v>
       </c>
       <c r="K51" s="42"/>
-      <c r="L51" s="40">
-        <v>1</v>
-      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="60"/>
+      <c r="A60" s="59"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="60"/>
+      <c r="A61" s="59"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="60"/>
+      <c r="A62" s="59"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="60"/>
+      <c r="A63" s="59"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="12"/>
@@ -4203,13 +4264,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A19:A41"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A50:A51"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:A17"/>
@@ -4217,59 +4271,102 @@
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A19:A40"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A50:A51"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <conditionalFormatting sqref="D68:D69">
-    <cfRule type="cellIs" dxfId="28" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="157" operator="equal">
       <formula>"Implemented"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:D69">
-    <cfRule type="cellIs" dxfId="27" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="156" operator="equal">
       <formula>"Under implementation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="cellIs" dxfId="26" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="154" operator="equal">
       <formula>"Note"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="155" operator="equal">
       <formula>"Discard"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G6 G50:G1048576 G8:G48">
-    <cfRule type="cellIs" dxfId="24" priority="80" operator="equal">
+  <conditionalFormatting sqref="G1:G6 G50:G1048576 G42:G48 G8:G40">
+    <cfRule type="cellIs" dxfId="34" priority="90" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="91" operator="equal">
       <formula>"Note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F6 F50:F1048576 F8:F48">
-    <cfRule type="cellIs" dxfId="22" priority="70" operator="equal">
+  <conditionalFormatting sqref="F1:F6 F50:F1048576 F42:F48 F8:F40">
+    <cfRule type="cellIs" dxfId="32" priority="80" operator="equal">
       <formula>"Draft"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="81" operator="equal">
       <formula>"In the work queue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="82" operator="equal">
       <formula>"Definition Ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="83" operator="equal">
       <formula>"Under implementation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="84" operator="equal">
       <formula>"Deletion"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="85" operator="equal">
       <formula>"Disabled"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="86" operator="equal">
       <formula>"Implemented"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G6 G8:G1048576">
-    <cfRule type="cellIs" dxfId="15" priority="51" operator="equal">
+  <conditionalFormatting sqref="G1:G6 G42:G1048576 G8:G40">
+    <cfRule type="cellIs" dxfId="25" priority="61" operator="equal">
+      <formula>"FIXED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+      <formula>"Note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+      <formula>"Draft"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+      <formula>"In the work queue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+      <formula>"Definition Ready"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+      <formula>"Under implementation"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+      <formula>"Deletion"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+      <formula>"Disabled"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+      <formula>"Implemented"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"FIXED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4293,7 +4390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3422C2F-3685-4409-95B8-394A1C678CE6}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -4315,7 +4412,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4353,7 +4450,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -4368,8 +4465,8 @@
       <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="60" t="s">
-        <v>168</v>
+      <c r="A3" s="59" t="s">
+        <v>135</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="9"/>
@@ -4383,7 +4480,7 @@
       <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="3"/>
       <c r="C4" s="9"/>
       <c r="E4" s="4"/>
@@ -4396,7 +4493,7 @@
       <c r="L4" s="23"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="3"/>
       <c r="C5" s="9"/>
       <c r="E5" s="4"/>
@@ -4409,7 +4506,7 @@
       <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="3"/>
       <c r="C6" s="9"/>
       <c r="E6" s="8"/>
@@ -4422,7 +4519,7 @@
       <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="60"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="3"/>
       <c r="C7" s="9"/>
       <c r="E7" s="4"/>
@@ -4435,7 +4532,7 @@
       <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="60"/>
+      <c r="A8" s="59"/>
       <c r="C8" s="9"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -4447,7 +4544,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="61"/>
@@ -4462,8 +4559,8 @@
       <c r="L9" s="22"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="60" t="s">
-        <v>214</v>
+      <c r="A10" s="59" t="s">
+        <v>176</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4477,7 +4574,7 @@
       <c r="L10" s="23"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="60"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="E11" s="4"/>
@@ -4490,7 +4587,7 @@
       <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="60"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="E12" s="4"/>
@@ -4503,7 +4600,7 @@
       <c r="L12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="E13" s="4"/>
@@ -4516,7 +4613,7 @@
       <c r="L13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="60"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="E14" s="4"/>
@@ -4529,7 +4626,7 @@
       <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="E15" s="4"/>
@@ -4542,7 +4639,7 @@
       <c r="L15" s="23"/>
     </row>
     <row r="16" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="60"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="E16" s="4"/>
@@ -4556,7 +4653,7 @@
     </row>
     <row r="17" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="61" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B17" s="61"/>
       <c r="C17" s="61"/>
@@ -4571,8 +4668,8 @@
       <c r="L17" s="22"/>
     </row>
     <row r="18" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="60" t="s">
-        <v>169</v>
+      <c r="A18" s="59" t="s">
+        <v>136</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4586,7 +4683,7 @@
       <c r="L18" s="23"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="60"/>
+      <c r="A19" s="59"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="E19" s="4"/>
@@ -4599,7 +4696,7 @@
       <c r="L19" s="23"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="60"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="E20" s="4"/>
@@ -4612,7 +4709,7 @@
       <c r="L20" s="23"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="60"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="E21" s="4"/>
@@ -4625,7 +4722,7 @@
       <c r="L21" s="23"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="60"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="E22" s="4"/>
@@ -4638,7 +4735,7 @@
       <c r="L22" s="23"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="60"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="E23" s="4"/>
@@ -4651,7 +4748,7 @@
       <c r="L23" s="23"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="60"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="17"/>
       <c r="C24" s="3"/>
       <c r="E24" s="6"/>
@@ -4664,7 +4761,7 @@
       <c r="L24" s="23"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="17"/>
       <c r="C25" s="3"/>
       <c r="E25" s="6"/>
@@ -4677,7 +4774,7 @@
       <c r="L25" s="23"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="17"/>
       <c r="C26" s="3"/>
       <c r="E26" s="6"/>
@@ -4690,7 +4787,7 @@
       <c r="L26" s="23"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="60"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="17"/>
       <c r="C27" s="3"/>
       <c r="E27" s="6"/>
@@ -4703,7 +4800,7 @@
       <c r="L27" s="23"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="60"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="17"/>
       <c r="C28" s="3"/>
       <c r="E28" s="6"/>
@@ -4716,7 +4813,7 @@
       <c r="L28" s="23"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="60"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="17"/>
       <c r="C29" s="3"/>
       <c r="E29" s="6"/>
@@ -4729,7 +4826,7 @@
       <c r="L29" s="23"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="17"/>
       <c r="C30" s="3"/>
       <c r="E30" s="6"/>
@@ -4742,7 +4839,7 @@
       <c r="L30" s="23"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="60"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="17"/>
       <c r="C31" s="3"/>
       <c r="E31" s="4"/>
@@ -4755,7 +4852,7 @@
       <c r="L31" s="23"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="60"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="17"/>
       <c r="C32" s="3"/>
       <c r="E32" s="4"/>
@@ -4768,7 +4865,7 @@
       <c r="L32" s="23"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="60"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="17"/>
       <c r="C33" s="3"/>
       <c r="E33" s="4"/>
@@ -4781,7 +4878,7 @@
       <c r="L33" s="23"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="60"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="17"/>
       <c r="C34" s="3"/>
       <c r="E34" s="4"/>
@@ -4794,7 +4891,7 @@
       <c r="L34" s="23"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="60"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="17"/>
       <c r="C35" s="3"/>
       <c r="E35" s="4"/>
@@ -4807,7 +4904,7 @@
       <c r="L35" s="23"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="60"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="17"/>
       <c r="C36" s="12"/>
       <c r="E36" s="4"/>
@@ -4820,7 +4917,7 @@
       <c r="L36" s="23"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="60"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="3"/>
       <c r="C37" s="12"/>
       <c r="E37" s="10"/>
@@ -4833,7 +4930,7 @@
       <c r="L37" s="23"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="60"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="3"/>
       <c r="C38" s="12"/>
       <c r="E38" s="10"/>
@@ -4846,7 +4943,7 @@
       <c r="L38" s="23"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="17"/>
       <c r="C39" s="3"/>
       <c r="E39" s="4"/>
@@ -4859,7 +4956,7 @@
       <c r="L39" s="23"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="60"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="17"/>
       <c r="C40" s="3"/>
       <c r="E40" s="4"/>
@@ -4873,7 +4970,7 @@
     </row>
     <row r="41" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="61" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -4888,8 +4985,8 @@
       <c r="L41" s="22"/>
     </row>
     <row r="42" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="60" t="s">
-        <v>170</v>
+      <c r="A42" s="59" t="s">
+        <v>137</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -4904,7 +5001,7 @@
       <c r="L42" s="23"/>
     </row>
     <row r="43" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="60"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="8"/>
@@ -4918,7 +5015,7 @@
       <c r="L43" s="23"/>
     </row>
     <row r="44" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="60"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="8"/>
@@ -4932,7 +5029,7 @@
       <c r="L44" s="23"/>
     </row>
     <row r="45" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="60"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="8"/>
@@ -4946,7 +5043,7 @@
       <c r="L45" s="23"/>
     </row>
     <row r="46" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="60"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="8"/>
@@ -4960,7 +5057,7 @@
       <c r="L46" s="23"/>
     </row>
     <row r="47" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="60"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="8"/>
@@ -4975,7 +5072,7 @@
     </row>
     <row r="48" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="61" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="B48" s="61"/>
       <c r="C48" s="13"/>
@@ -4990,8 +5087,8 @@
       <c r="L48" s="22"/>
     </row>
     <row r="49" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="60" t="s">
-        <v>213</v>
+      <c r="A49" s="59" t="s">
+        <v>175</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -5002,7 +5099,7 @@
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:12" s="25" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="60"/>
+      <c r="A50" s="59"/>
       <c r="B50" s="26"/>
       <c r="C50" s="3"/>
       <c r="D50" s="8"/>
@@ -5016,7 +5113,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="30" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="13"/>
@@ -5031,8 +5128,8 @@
       <c r="L51" s="22"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="60" t="s">
-        <v>212</v>
+      <c r="A52" s="59" t="s">
+        <v>174</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>
@@ -5045,7 +5142,7 @@
       <c r="K52" s="18"/>
     </row>
     <row r="53" spans="1:12" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="60"/>
+      <c r="A53" s="59"/>
       <c r="C53" s="3"/>
       <c r="D53" s="4"/>
       <c r="E53" s="27"/>
@@ -5057,16 +5154,16 @@
       <c r="K53" s="18"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="60"/>
+      <c r="A62" s="59"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="60"/>
+      <c r="A63" s="59"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="60"/>
+      <c r="A64" s="59"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="60"/>
+      <c r="A65" s="59"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70" s="3"/>
@@ -5092,18 +5189,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A18:A40"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A17:J17"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="A42:A47"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="A62:A65"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A18:A40"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <conditionalFormatting sqref="D70:D71">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">

</xml_diff>